<commit_message>
finally combined everything, final result gui pending creation
</commit_message>
<xml_diff>
--- a/Codes/Subchannel Analysis/GUI/gooddata.xlsx
+++ b/Codes/Subchannel Analysis/GUI/gooddata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\COde work\Things\Subchannel-Analysis\Codes\Subchannel Analysis\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088E9345-D267-4D2A-95F0-FD61A39D2BE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0495B7-78F7-4EF0-9F6D-1E9ECEEBAA56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C11">
         <v>4.1399999999999996E-3</v>

</xml_diff>

<commit_message>
final GUI complete with plotting
</commit_message>
<xml_diff>
--- a/Codes/Subchannel Analysis/GUI/gooddata.xlsx
+++ b/Codes/Subchannel Analysis/GUI/gooddata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\COde work\Things\Subchannel-Analysis\Codes\Subchannel Analysis\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0495B7-78F7-4EF0-9F6D-1E9ECEEBAA56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2552903-2E1E-41A0-9C25-5EBFC3EDC945}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>4.1399999999999996E-3</v>

</xml_diff>